<commit_message>
Bug Fixes in Log in
</commit_message>
<xml_diff>
--- a/MasterList.xlsx
+++ b/MasterList.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="29">
   <si>
     <t>Student Number</t>
   </si>
@@ -82,6 +82,36 @@
   </si>
   <si>
     <t>Math</t>
+  </si>
+  <si>
+    <t>4:54 PM</t>
+  </si>
+  <si>
+    <t>Yash</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>4:58 PM</t>
+  </si>
+  <si>
+    <t>222222222</t>
+  </si>
+  <si>
+    <t>Guy</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Academic Support</t>
+  </si>
+  <si>
+    <t>4:59 PM</t>
+  </si>
+  <si>
+    <t>Chill Zone</t>
   </si>
 </sst>
 </file>
@@ -434,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB36B92-3664-F44C-863F-9EAE1729DA0F}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
@@ -508,6 +538,98 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>